<commit_message>
finished V2.1 output will be as default as xlsx , and json will be optional
</commit_message>
<xml_diff>
--- a/ASINs/B07MW4BR8D.xlsx
+++ b/ASINs/B07MW4BR8D.xlsx
@@ -9,14 +9,13 @@
   <sheets>
     <sheet name="Product_Profile" sheetId="1" r:id="rId1"/>
     <sheet name="Product_Reviews" sheetId="2" r:id="rId2"/>
-    <sheet name="Product_Questions" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="106">
   <si>
     <t>Product_Profile</t>
   </si>
@@ -69,7 +68,7 @@
     <t>https://www.amazon.com/Heiyo-Magnetic-Rechargeable-Capacitive-Compatible/product-reviews/B07MW4BR8D/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews&amp;filterByStar=positive&amp;pageNumber=1</t>
   </si>
   <si>
-    <t>$27.99</t>
+    <t>None &lt;&lt; means not available</t>
   </si>
   <si>
     <t>https://www.amazon.com/ask/questions/asin/B07MW4BR8D/</t>
@@ -337,78 +336,6 @@
   </si>
   <si>
     <t>Review_ASIN_</t>
-  </si>
-  <si>
-    <t>Question_</t>
-  </si>
-  <si>
-    <t>Given that this pen uses a rubber nib at the tip and doesn't connect wirelessly to your device, why does the pen need to be charged?</t>
-  </si>
-  <si>
-    <t>How is the quality of it?</t>
-  </si>
-  <si>
-    <t>Will this work for my touch screen HP notebook laptop?</t>
-  </si>
-  <si>
-    <t>does this support windows right-click?</t>
-  </si>
-  <si>
-    <t>does this work with the hp chromebook x360 14b?</t>
-  </si>
-  <si>
-    <t>Will this stylus work with the nintendo switch? with games like super mario maker and the level editor for ssbu, it would be nice to have a stylus.</t>
-  </si>
-  <si>
-    <t>Will it scratch my screen?</t>
-  </si>
-  <si>
-    <t>Is it good for mate 20 pro?</t>
-  </si>
-  <si>
-    <t>Is there a warranty on the heiyo stylus pen with magnetic charging station, 30-day standby &amp; 10 hrs using time rechargeable capacitive digital pen com</t>
-  </si>
-  <si>
-    <t>Will this stylus pen work with the samsung galaxy tab 3 (9.7)?</t>
-  </si>
-  <si>
-    <t>Answer_</t>
-  </si>
-  <si>
-    <t>dear, it do not any connect, you just touch your iphone or ipad ,it can work.</t>
-  </si>
-  <si>
-    <t>Good quality. But the tip is copper. It may scratch the screen over time if you do not have a screen protector.</t>
-  </si>
-  <si>
-    <t>Ive used this on my ipad, note 8 and touch screen windows 10 laptop with no problem</t>
-  </si>
-  <si>
-    <t>The pen acts the same as your finger, where “left click“ is a tap and “right click” is accessed by long-pressing the pen (or finger) and the menu pops up.</t>
-  </si>
-  <si>
-    <t>If it is touchscreen, yes.</t>
-  </si>
-  <si>
-    <t>dear, this pen only as a stylus pen, it do not need any connection, as long as your figer can work, this pen can work for your devices.</t>
-  </si>
-  <si>
-    <t>Over time yes if you do not have a screen protector. The tips is copper.</t>
-  </si>
-  <si>
-    <t>dear, as long as you rfinger can work for your phone, our stylus pen can work</t>
-  </si>
-  <si>
-    <t>don’t know about warranties - always best to directly ask mfg. because that info can change.
-I do know it is a really nice stylus for the price.</t>
-  </si>
-  <si>
-    <t>Dear,
-This iPad pen is designed for iPad series, but we haven't test it on Samsung Galaxy series.
-if you have any question, you can contact with our service team</t>
-  </si>
-  <si>
-    <t>Question_ASIN_</t>
   </si>
 </sst>
 </file>
@@ -1514,138 +1441,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>114</v>
-      </c>
-      <c r="B9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>